<commit_message>
add check of empty field for input
</commit_message>
<xml_diff>
--- a/eq_log/eq_file/80001840.xlsx
+++ b/eq_log/eq_file/80001840.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -81,6 +81,126 @@
   </si>
   <si>
     <t>8</t>
+  </si>
+  <si>
+    <t>27/03/2018</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
   </si>
   <si>
     <t>**</t>
@@ -893,6 +1013,15 @@
       <c r="A11" t="s">
         <v>22</v>
       </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
       <c r="E11" s="24">
         <f>D11-D10</f>
         <v/>
@@ -901,6 +1030,18 @@
       <c r="H11" s="17" t="n"/>
     </row>
     <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
       <c r="E12" s="24">
         <f>D12-D11</f>
         <v/>
@@ -910,6 +1051,18 @@
       <c r="H12" s="17" t="n"/>
     </row>
     <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
       <c r="E13" s="24">
         <f>D13-D12</f>
         <v/>
@@ -919,6 +1072,18 @@
       <c r="H13" s="17" t="n"/>
     </row>
     <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
       <c r="E14" s="24">
         <f>D14-D13</f>
         <v/>
@@ -928,6 +1093,18 @@
       <c r="H14" s="17" t="n"/>
     </row>
     <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
       <c r="E15" s="24">
         <f>D15-D14</f>
         <v/>
@@ -937,6 +1114,18 @@
       <c r="H15" s="17" t="n"/>
     </row>
     <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
       <c r="E16" s="24">
         <f>D16-D15</f>
         <v/>
@@ -946,6 +1135,18 @@
       <c r="H16" s="17" t="n"/>
     </row>
     <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
       <c r="E17" s="24">
         <f>D17-D16</f>
         <v/>
@@ -955,6 +1156,18 @@
       <c r="H17" s="17" t="n"/>
     </row>
     <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
       <c r="E18" s="24">
         <f>D18-D17</f>
         <v/>
@@ -964,6 +1177,18 @@
       <c r="H18" s="17" t="n"/>
     </row>
     <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
       <c r="E19" s="24">
         <f>D19-D18</f>
         <v/>
@@ -973,6 +1198,18 @@
       <c r="H19" s="17" t="n"/>
     </row>
     <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
+      </c>
       <c r="E20" s="24">
         <f>D20-D19</f>
         <v/>
@@ -982,6 +1219,18 @@
       <c r="H20" s="17" t="n"/>
     </row>
     <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
       <c r="E21" s="24">
         <f>D21-D20</f>
         <v/>
@@ -991,6 +1240,18 @@
       <c r="H21" s="17" t="n"/>
     </row>
     <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
       <c r="E22" s="24">
         <f>D22-D21</f>
         <v/>
@@ -1000,6 +1261,18 @@
       <c r="H22" s="17" t="n"/>
     </row>
     <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
       <c r="E23" s="24">
         <f>D23-D22</f>
         <v/>
@@ -1009,6 +1282,18 @@
       <c r="H23" s="17" t="n"/>
     </row>
     <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
       <c r="E24" s="24">
         <f>D24-D23</f>
         <v/>
@@ -1017,6 +1302,18 @@
       <c r="H24" s="17" t="n"/>
     </row>
     <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
       <c r="E25" s="24">
         <f>D25-D24</f>
         <v/>
@@ -1025,6 +1322,18 @@
       <c r="H25" s="17" t="n"/>
     </row>
     <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
       <c r="E26" s="24">
         <f>D26-D25</f>
         <v/>
@@ -1032,6 +1341,18 @@
       <c r="F26" s="10" t="n"/>
     </row>
     <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
       <c r="E27" s="24">
         <f>D27-D26</f>
         <v/>
@@ -1039,6 +1360,18 @@
       <c r="F27" s="10" t="n"/>
     </row>
     <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" t="s">
+        <v>40</v>
+      </c>
       <c r="E28" s="24">
         <f>D28-D27</f>
         <v/>
@@ -1046,6 +1379,18 @@
       <c r="F28" s="10" t="n"/>
     </row>
     <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
+        <v>41</v>
+      </c>
       <c r="E29" s="24">
         <f>D29-D28</f>
         <v/>
@@ -1053,6 +1398,18 @@
       <c r="F29" s="10" t="n"/>
     </row>
     <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
       <c r="E30" s="24">
         <f>D30-D29</f>
         <v/>
@@ -1060,6 +1417,18 @@
       <c r="F30" s="10" t="n"/>
     </row>
     <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
       <c r="E31" s="24">
         <f>D31-D30</f>
         <v/>
@@ -1067,6 +1436,18 @@
       <c r="F31" s="10" t="n"/>
     </row>
     <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
       <c r="E32" s="24">
         <f>D32-D31</f>
         <v/>
@@ -1074,6 +1455,18 @@
       <c r="F32" s="10" t="n"/>
     </row>
     <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" t="s">
+        <v>45</v>
+      </c>
       <c r="E33" s="24">
         <f>D33-D32</f>
         <v/>
@@ -1081,6 +1474,18 @@
       <c r="F33" s="10" t="n"/>
     </row>
     <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" t="s">
+        <v>46</v>
+      </c>
       <c r="E34" s="24">
         <f>D34-D33</f>
         <v/>
@@ -1088,6 +1493,18 @@
       <c r="F34" s="10" t="n"/>
     </row>
     <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" t="s">
+        <v>47</v>
+      </c>
       <c r="E35" s="24">
         <f>D35-D34</f>
         <v/>
@@ -1095,6 +1512,18 @@
       <c r="F35" s="10" t="n"/>
     </row>
     <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" t="s">
+        <v>48</v>
+      </c>
       <c r="E36" s="24">
         <f>D36-D35</f>
         <v/>
@@ -1102,6 +1531,18 @@
       <c r="F36" s="10" t="n"/>
     </row>
     <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
       <c r="E37" s="24">
         <f>D37-D36</f>
         <v/>
@@ -1109,6 +1550,18 @@
       <c r="F37" s="10" t="n"/>
     </row>
     <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
+        <v>50</v>
+      </c>
       <c r="E38" s="24">
         <f>D38-D37</f>
         <v/>
@@ -1116,6 +1569,18 @@
       <c r="F38" s="10" t="n"/>
     </row>
     <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" t="s">
+        <v>51</v>
+      </c>
       <c r="E39" s="24">
         <f>D39-D38</f>
         <v/>
@@ -1123,6 +1588,18 @@
       <c r="F39" s="10" t="n"/>
     </row>
     <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s">
+        <v>52</v>
+      </c>
       <c r="E40" s="24">
         <f>D40-D39</f>
         <v/>
@@ -1130,6 +1607,18 @@
       <c r="F40" s="10" t="n"/>
     </row>
     <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" t="s">
+        <v>53</v>
+      </c>
       <c r="E41" s="24">
         <f>D41-D40</f>
         <v/>
@@ -1137,6 +1626,18 @@
       <c r="F41" s="10" t="n"/>
     </row>
     <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
+        <v>54</v>
+      </c>
       <c r="E42" s="24">
         <f>D42-D41</f>
         <v/>
@@ -1144,6 +1645,18 @@
       <c r="F42" s="10" t="n"/>
     </row>
     <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" t="s">
+        <v>55</v>
+      </c>
       <c r="E43" s="24">
         <f>D43-D42</f>
         <v/>
@@ -1151,6 +1664,18 @@
       <c r="F43" s="10" t="n"/>
     </row>
     <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" t="s">
+        <v>56</v>
+      </c>
       <c r="E44" s="24">
         <f>D44-D43</f>
         <v/>
@@ -1158,6 +1683,18 @@
       <c r="F44" s="10" t="n"/>
     </row>
     <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" t="s">
+        <v>57</v>
+      </c>
       <c r="E45" s="24">
         <f>D45-D44</f>
         <v/>
@@ -1165,6 +1702,18 @@
       <c r="F45" s="10" t="n"/>
     </row>
     <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" t="s">
+        <v>58</v>
+      </c>
       <c r="E46" s="24">
         <f>D46-D45</f>
         <v/>
@@ -1172,6 +1721,18 @@
       <c r="F46" s="10" t="n"/>
     </row>
     <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" t="s">
+        <v>59</v>
+      </c>
       <c r="E47" s="24">
         <f>D47-D46</f>
         <v/>
@@ -1179,6 +1740,18 @@
       <c r="F47" s="10" t="n"/>
     </row>
     <row r="48" spans="1:9">
+      <c r="A48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" t="s">
+        <v>60</v>
+      </c>
       <c r="E48" s="24">
         <f>D48-D47</f>
         <v/>
@@ -1186,6 +1759,18 @@
       <c r="F48" s="10" t="n"/>
     </row>
     <row r="49" spans="1:9">
+      <c r="A49" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" t="s">
+        <v>61</v>
+      </c>
       <c r="E49" s="24">
         <f>D49-D48</f>
         <v/>
@@ -1193,6 +1778,9 @@
       <c r="F49" s="10" t="n"/>
     </row>
     <row r="50" spans="1:9">
+      <c r="A50" t="s">
+        <v>62</v>
+      </c>
       <c r="E50" s="24">
         <f>D50-D49</f>
         <v/>
@@ -49855,21 +50443,21 @@
   <sheetData>
     <row customFormat="1" r="1" s="18" spans="1:6">
       <c r="A1" s="19" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="25" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="D3" s="25">
         <f>C3-C2</f>

</xml_diff>

<commit_message>
fix field of mistake input
</commit_message>
<xml_diff>
--- a/eq_log/eq_file/80001840.xlsx
+++ b/eq_log/eq_file/80001840.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -201,6 +201,15 @@
   </si>
   <si>
     <t>49</t>
+  </si>
+  <si>
+    <t>28/03/2018</t>
+  </si>
+  <si>
+    <t>Не відповідне скручення проводів</t>
+  </si>
+  <si>
+    <t>50</t>
   </si>
   <si>
     <t>**</t>
@@ -1781,6 +1790,15 @@
       <c r="A50" t="s">
         <v>62</v>
       </c>
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" t="s">
+        <v>64</v>
+      </c>
       <c r="E50" s="24">
         <f>D50-D49</f>
         <v/>
@@ -1788,6 +1806,9 @@
       <c r="F50" s="10" t="n"/>
     </row>
     <row r="51" spans="1:9">
+      <c r="A51" t="s">
+        <v>65</v>
+      </c>
       <c r="E51" s="24">
         <f>D51-D50</f>
         <v/>
@@ -50443,21 +50464,21 @@
   <sheetData>
     <row customFormat="1" r="1" s="18" spans="1:6">
       <c r="A1" s="19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="25" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D3" s="25">
         <f>C3-C2</f>

</xml_diff>

<commit_message>
fix sumcalculation for ecxel file
</commit_message>
<xml_diff>
--- a/eq_log/eq_file/80001840.xlsx
+++ b/eq_log/eq_file/80001840.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="88">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -255,6 +255,15 @@
   </si>
   <si>
     <t>65</t>
+  </si>
+  <si>
+    <t>Пошкодження поверхні контакту</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
   </si>
   <si>
     <t>**</t>
@@ -2118,7 +2127,16 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" t="s">
         <v>80</v>
+      </c>
+      <c r="D65" t="s">
+        <v>81</v>
       </c>
       <c r="E65" s="24">
         <f>D65-D64</f>
@@ -2127,6 +2145,18 @@
       <c r="F65" s="10" t="n"/>
     </row>
     <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
+        <v>80</v>
+      </c>
+      <c r="D66" t="s">
+        <v>82</v>
+      </c>
       <c r="E66" s="24">
         <f>D66-D65</f>
         <v/>
@@ -2134,6 +2164,9 @@
       <c r="F66" s="10" t="n"/>
     </row>
     <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>83</v>
+      </c>
       <c r="E67" s="24">
         <f>D67-D66</f>
         <v/>
@@ -50677,21 +50710,21 @@
   <sheetData>
     <row customFormat="1" r="1" s="18" spans="1:6">
       <c r="A1" s="19" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="25" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D3" s="25">
         <f>C3-C2</f>

</xml_diff>

<commit_message>
totaly fix sumcalculation for ecxel file
</commit_message>
<xml_diff>
--- a/eq_log/eq_file/80001840.xlsx
+++ b/eq_log/eq_file/80001840.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -264,6 +264,12 @@
   </si>
   <si>
     <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>69</t>
   </si>
   <si>
     <t>**</t>
@@ -2165,6 +2171,15 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" t="s">
         <v>83</v>
       </c>
       <c r="E67" s="24">
@@ -2174,6 +2189,18 @@
       <c r="F67" s="10" t="n"/>
     </row>
     <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" t="s">
+        <v>84</v>
+      </c>
       <c r="E68" s="24">
         <f>D68-D67</f>
         <v/>
@@ -2181,6 +2208,9 @@
       <c r="F68" s="10" t="n"/>
     </row>
     <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>85</v>
+      </c>
       <c r="E69" s="24">
         <f>D69-D68</f>
         <v/>
@@ -50710,21 +50740,21 @@
   <sheetData>
     <row customFormat="1" r="1" s="18" spans="1:6">
       <c r="A1" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D3" s="25">
         <f>C3-C2</f>

</xml_diff>